<commit_message>
Scenario for Create account using Excel Data Read
</commit_message>
<xml_diff>
--- a/CrossplatformApp/TestDataWestband.xlsx
+++ b/CrossplatformApp/TestDataWestband.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19155" windowHeight="8520"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19155" windowHeight="8520" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="RegistrationData" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Userid</t>
   </si>
@@ -64,6 +64,72 @@
   </si>
   <si>
     <t>This id contains Many data</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Contact no</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Lokesh</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>lokesh400@xtivia.com</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ValidData</t>
+  </si>
+  <si>
+    <t>lokesh401@xtivia.com</t>
+  </si>
+  <si>
+    <t>Invalid Data</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Name Cant be blank</t>
+  </si>
+  <si>
+    <t>lokesh402@xtivia.com</t>
+  </si>
+  <si>
+    <t>LastName cant be blank</t>
+  </si>
+  <si>
+    <t>Email Cant be blank</t>
+  </si>
+  <si>
+    <t>lokesh403@xtivia.com</t>
+  </si>
+  <si>
+    <t>Gemini@251522</t>
+  </si>
+  <si>
+    <t>Password not matched</t>
+  </si>
+  <si>
+    <t>Lokeshsssss</t>
   </si>
 </sst>
 </file>
@@ -95,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +171,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,7 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -146,6 +218,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -450,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -550,13 +625,302 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8447520166</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8447520166</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3">
+        <v>8447520166</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>8447520166</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8447520166</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId6"/>
+    <hyperlink ref="E4" r:id="rId7"/>
+    <hyperlink ref="F3" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId9"/>
+    <hyperlink ref="E5" r:id="rId10"/>
+    <hyperlink ref="F5" r:id="rId11"/>
+    <hyperlink ref="C6" r:id="rId12"/>
+    <hyperlink ref="E6" r:id="rId13"/>
+    <hyperlink ref="F6" r:id="rId14"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Commit latest code for create accunt
</commit_message>
<xml_diff>
--- a/CrossplatformApp/TestDataWestband.xlsx
+++ b/CrossplatformApp/TestDataWestband.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Userid</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Lokeshsssss</t>
+  </si>
+  <si>
+    <t>Need to provide data</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,9 +779,7 @@
       <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3">
-        <v>8447520166</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
@@ -797,10 +798,18 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="E7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -918,9 +927,11 @@
     <hyperlink ref="C6" r:id="rId12"/>
     <hyperlink ref="E6" r:id="rId13"/>
     <hyperlink ref="F6" r:id="rId14"/>
+    <hyperlink ref="E7" r:id="rId15"/>
+    <hyperlink ref="F7" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create Account working code
</commit_message>
<xml_diff>
--- a/CrossplatformApp/TestDataWestband.xlsx
+++ b/CrossplatformApp/TestDataWestband.xlsx
@@ -75,9 +75,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Contact no</t>
-  </si>
-  <si>
     <t>ConfirmPassword</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Need to provide data</t>
+  </si>
+  <si>
+    <t>Contact</t>
   </si>
 </sst>
 </file>
@@ -631,15 +631,15 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16" customWidth="1"/>
+    <col min="3" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -656,32 +656,32 @@
         <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>8447520166</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -691,71 +691,69 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8447520166</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3">
-        <v>8447520166</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8447520166</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" s="3">
-        <v>8447520166</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>8447520166</v>
-      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
@@ -763,34 +761,36 @@
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8447520166</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,13 +802,13 @@
         <v>3</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,9 +929,11 @@
     <hyperlink ref="F6" r:id="rId14"/>
     <hyperlink ref="E7" r:id="rId15"/>
     <hyperlink ref="F7" r:id="rId16"/>
+    <hyperlink ref="D2:D4" r:id="rId17" display="lokesh403@xtivia.com"/>
+    <hyperlink ref="D6" r:id="rId18" display="lokesh403@xtivia.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create Account Mobile scenario with Updated Test records
</commit_message>
<xml_diff>
--- a/CrossplatformApp/TestDataWestband.xlsx
+++ b/CrossplatformApp/TestDataWestband.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Userid</t>
   </si>
@@ -78,61 +78,73 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ValidData</t>
+  </si>
+  <si>
+    <t>lokesh401@xtivia.com</t>
+  </si>
+  <si>
+    <t>Invalid Data</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Name Cant be blank</t>
+  </si>
+  <si>
+    <t>lokesh402@xtivia.com</t>
+  </si>
+  <si>
+    <t>LastName cant be blank</t>
+  </si>
+  <si>
+    <t>Email Cant be blank</t>
+  </si>
+  <si>
+    <t>lokesh403@xtivia.com</t>
+  </si>
+  <si>
+    <t>Gemini@251522</t>
+  </si>
+  <si>
+    <t>Password not matched</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Sharma2</t>
+  </si>
+  <si>
+    <t>Lokesh3</t>
+  </si>
+  <si>
+    <t>Lokesh4</t>
+  </si>
+  <si>
+    <t>Lokesh5</t>
+  </si>
+  <si>
+    <t>Sharma4</t>
+  </si>
+  <si>
+    <t>Sharma5</t>
+  </si>
+  <si>
+    <t>lokesh405@xtivia.com</t>
+  </si>
+  <si>
     <t>Lokesh</t>
-  </si>
-  <si>
-    <t>Sharma</t>
-  </si>
-  <si>
-    <t>lokesh400@xtivia.com</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>ValidData</t>
-  </si>
-  <si>
-    <t>lokesh401@xtivia.com</t>
-  </si>
-  <si>
-    <t>Invalid Data</t>
-  </si>
-  <si>
-    <t>ErrorMessage</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Name Cant be blank</t>
-  </si>
-  <si>
-    <t>lokesh402@xtivia.com</t>
-  </si>
-  <si>
-    <t>LastName cant be blank</t>
-  </si>
-  <si>
-    <t>Email Cant be blank</t>
-  </si>
-  <si>
-    <t>lokesh403@xtivia.com</t>
-  </si>
-  <si>
-    <t>Gemini@251522</t>
-  </si>
-  <si>
-    <t>Password not matched</t>
-  </si>
-  <si>
-    <t>Lokeshsssss</t>
-  </si>
-  <si>
-    <t>Need to provide data</t>
-  </si>
-  <si>
-    <t>Contact</t>
   </si>
 </sst>
 </file>
@@ -529,7 +541,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,10 +640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +668,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -665,21 +677,21 @@
         <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5">
         <v>8447520166</v>
@@ -691,19 +703,19 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D3" s="5">
         <v>8447520166</v>
@@ -715,19 +727,19 @@
         <v>3</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="5">
         <v>8447520166</v>
@@ -739,21 +751,23 @@
         <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <v>8447520166</v>
+      </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
@@ -761,36 +775,34 @@
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8447520166</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -798,18 +810,10 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -900,16 +904,6 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -927,13 +921,11 @@
     <hyperlink ref="C6" r:id="rId12"/>
     <hyperlink ref="E6" r:id="rId13"/>
     <hyperlink ref="F6" r:id="rId14"/>
-    <hyperlink ref="E7" r:id="rId15"/>
-    <hyperlink ref="F7" r:id="rId16"/>
-    <hyperlink ref="D2:D4" r:id="rId17" display="lokesh403@xtivia.com"/>
-    <hyperlink ref="D6" r:id="rId18" display="lokesh403@xtivia.com"/>
+    <hyperlink ref="D2:D4" r:id="rId15" display="lokesh403@xtivia.com"/>
+    <hyperlink ref="D5" r:id="rId16" display="lokesh403@xtivia.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create account Password not matched scenario
</commit_message>
<xml_diff>
--- a/CrossplatformApp/TestDataWestband.xlsx
+++ b/CrossplatformApp/TestDataWestband.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Userid</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Lokesh</t>
+  </si>
+  <si>
+    <t>lokesh406@xtivia.com</t>
+  </si>
+  <si>
+    <t>Checkbox not clicked</t>
   </si>
 </sst>
 </file>
@@ -643,7 +649,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,24 +802,40 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="5">
+        <v>8447520166</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -923,9 +945,13 @@
     <hyperlink ref="F6" r:id="rId14"/>
     <hyperlink ref="D2:D4" r:id="rId15" display="lokesh403@xtivia.com"/>
     <hyperlink ref="D5" r:id="rId16" display="lokesh403@xtivia.com"/>
+    <hyperlink ref="C7" r:id="rId17"/>
+    <hyperlink ref="D7" r:id="rId18" display="lokesh403@xtivia.com"/>
+    <hyperlink ref="E7" r:id="rId19"/>
+    <hyperlink ref="F7" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create account Blank Password Scenario
</commit_message>
<xml_diff>
--- a/CrossplatformApp/TestDataWestband.xlsx
+++ b/CrossplatformApp/TestDataWestband.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>Userid</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Checkbox not clicked</t>
+  </si>
+  <si>
+    <t>lokesh407@xtivia.com</t>
+  </si>
+  <si>
+    <t>Password cant be blank</t>
   </si>
 </sst>
 </file>
@@ -649,7 +655,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,14 +844,26 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8447520166</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -949,9 +967,11 @@
     <hyperlink ref="D7" r:id="rId18" display="lokesh403@xtivia.com"/>
     <hyperlink ref="E7" r:id="rId19"/>
     <hyperlink ref="F7" r:id="rId20"/>
+    <hyperlink ref="C8" r:id="rId21"/>
+    <hyperlink ref="D8" r:id="rId22" display="lokesh403@xtivia.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Excel Utility changes:-Issue while open the excel sheet again and again , not opens --Fixed
</commit_message>
<xml_diff>
--- a/CrossplatformApp/TestDataWestband.xlsx
+++ b/CrossplatformApp/TestDataWestband.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Userid</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>Password cant be blank</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Wolinski</t>
+  </si>
+  <si>
+    <t>mwolinski@xtivia.com</t>
+  </si>
+  <si>
+    <t>ValidData but Email already exist</t>
+  </si>
+  <si>
+    <t>Email id already exist</t>
   </si>
 </sst>
 </file>
@@ -655,7 +670,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +680,7 @@
     <col min="3" max="4" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -866,14 +881,30 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8447520166</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -969,9 +1000,13 @@
     <hyperlink ref="F7" r:id="rId20"/>
     <hyperlink ref="C8" r:id="rId21"/>
     <hyperlink ref="D8" r:id="rId22" display="lokesh403@xtivia.com"/>
+    <hyperlink ref="C9" r:id="rId23"/>
+    <hyperlink ref="D9" r:id="rId24" display="lokesh403@xtivia.com"/>
+    <hyperlink ref="E9" r:id="rId25"/>
+    <hyperlink ref="F9" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>